<commit_message>
bug fix, reportData ready
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\762-impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97341DFB-C9CD-47C5-806D-6CA648AAC719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307B50BB-9245-41C2-93A3-5EBFC18B82C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="29445" yWindow="2115" windowWidth="20745" windowHeight="10515" xr2:uid="{37BDFEDE-B0AD-4CF0-AC3D-1AFBC0ABC248}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12645" xr2:uid="{37BDFEDE-B0AD-4CF0-AC3D-1AFBC0ABC248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Killing Excel Notepad and Edge if open Updated
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molin\300_Process\PHEV_Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7282FBA2-EAD1-49F7-A092-B2B03EFC38DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAA1F77-6D7B-4214-954A-A1EF45B05C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3670" windowWidth="7520" windowHeight="3370" xr2:uid="{CE13BDA5-F140-4DDF-A5DE-5622F27222D6}"/>
+    <workbookView xWindow="11270" yWindow="1900" windowWidth="7520" windowHeight="3370" xr2:uid="{FD5F6010-DD89-4094-ACBD-EB6F4160259C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="165">
   <si>
     <t>Make</t>
   </si>
@@ -95,396 +95,387 @@
     <t>renault</t>
   </si>
   <si>
+    <t>megane</t>
+  </si>
+  <si>
     <t>master</t>
   </si>
   <si>
+    <t>captur</t>
+  </si>
+  <si>
+    <t>peugeot</t>
+  </si>
+  <si>
+    <t>listing</t>
+  </si>
+  <si>
+    <t>triton</t>
+  </si>
+  <si>
+    <t>pajero</t>
+  </si>
+  <si>
+    <t>mirage</t>
+  </si>
+  <si>
+    <t>express</t>
+  </si>
+  <si>
+    <t>eclipse-cross</t>
+  </si>
+  <si>
+    <t>asx</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>land-rover</t>
+  </si>
+  <si>
+    <t>range-rover-velar</t>
+  </si>
+  <si>
+    <t>range-rover</t>
+  </si>
+  <si>
+    <t>kia</t>
+  </si>
+  <si>
+    <t>sorento</t>
+  </si>
+  <si>
+    <t>niro</t>
+  </si>
+  <si>
+    <t>isuzu</t>
+  </si>
+  <si>
+    <t>mu-x</t>
+  </si>
+  <si>
+    <t>d-max</t>
+  </si>
+  <si>
+    <t>hyundai</t>
+  </si>
+  <si>
+    <t>santa-fe</t>
+  </si>
+  <si>
+    <t>kona</t>
+  </si>
+  <si>
+    <t>ioniq-5</t>
+  </si>
+  <si>
+    <t>ioniq</t>
+  </si>
+  <si>
+    <t>i30</t>
+  </si>
+  <si>
+    <t>ford</t>
+  </si>
+  <si>
+    <t>transit</t>
+  </si>
+  <si>
+    <t>puma</t>
+  </si>
+  <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>citroen</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>byd</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>alfa-romeo</t>
+  </si>
+  <si>
+    <t>stelvio</t>
+  </si>
+  <si>
+    <t>t-roc</t>
+  </si>
+  <si>
+    <t>yaris</t>
+  </si>
+  <si>
+    <t>land-cruiser</t>
+  </si>
+  <si>
+    <t>highlander</t>
+  </si>
+  <si>
+    <t>mercedes-benz</t>
+  </si>
+  <si>
+    <t>e-300</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>staria</t>
+  </si>
+  <si>
+    <t>530e</t>
+  </si>
+  <si>
+    <t>supra</t>
+  </si>
+  <si>
+    <t>rav4</t>
+  </si>
+  <si>
+    <t>raize</t>
+  </si>
+  <si>
+    <t>hilux</t>
+  </si>
+  <si>
+    <t>porsche</t>
+  </si>
+  <si>
+    <t>cayenne</t>
+  </si>
+  <si>
+    <t>nissan</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>juke</t>
+  </si>
+  <si>
+    <t>honda</t>
+  </si>
+  <si>
+    <t>hr-v</t>
+  </si>
+  <si>
+    <t>fortuner</t>
+  </si>
+  <si>
+    <t>corolla</t>
+  </si>
+  <si>
     <t>koleos</t>
   </si>
   <si>
-    <t>kadjar</t>
-  </si>
-  <si>
-    <t>peugeot</t>
-  </si>
-  <si>
-    <t>listing</t>
-  </si>
-  <si>
-    <t>triton</t>
-  </si>
-  <si>
-    <t>pajero</t>
-  </si>
-  <si>
-    <t>mirage</t>
-  </si>
-  <si>
-    <t>express</t>
-  </si>
-  <si>
-    <t>eclipse-cross</t>
-  </si>
-  <si>
-    <t>asx</t>
-  </si>
-  <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>hs</t>
-  </si>
-  <si>
-    <t>land-rover</t>
-  </si>
-  <si>
-    <t>range-rover-velar</t>
+    <t>panamera</t>
+  </si>
+  <si>
+    <t>nv350</t>
+  </si>
+  <si>
+    <t>mazda</t>
+  </si>
+  <si>
+    <t>cx-30</t>
+  </si>
+  <si>
+    <t>range-rover-sport</t>
+  </si>
+  <si>
+    <t>seltos</t>
+  </si>
+  <si>
+    <t>tucson</t>
+  </si>
+  <si>
+    <t>accent</t>
+  </si>
+  <si>
+    <t>ranger</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>740e</t>
+  </si>
+  <si>
+    <t>golf</t>
+  </si>
+  <si>
+    <t>hiace</t>
+  </si>
+  <si>
+    <t>c-hr</t>
+  </si>
+  <si>
+    <t>aqua</t>
+  </si>
+  <si>
+    <t>mini</t>
+  </si>
+  <si>
+    <t>countryman</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>e-350</t>
+  </si>
+  <si>
+    <t>discovery-sport</t>
+  </si>
+  <si>
+    <t>audi</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>tiguan</t>
+  </si>
+  <si>
+    <t>vitz</t>
+  </si>
+  <si>
+    <t>subaru</t>
+  </si>
+  <si>
+    <t>xv</t>
+  </si>
+  <si>
+    <t>forester</t>
+  </si>
+  <si>
+    <t>c-350-e</t>
+  </si>
+  <si>
+    <t>cx-3</t>
+  </si>
+  <si>
+    <t>330e</t>
+  </si>
+  <si>
+    <t>polo</t>
+  </si>
+  <si>
+    <t>passat</t>
+  </si>
+  <si>
+    <t>land-cruiser-prado</t>
+  </si>
+  <si>
+    <t>sportage</t>
+  </si>
+  <si>
+    <t>225xe</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>jetta</t>
+  </si>
+  <si>
+    <t>camry</t>
+  </si>
+  <si>
+    <t>macan</t>
+  </si>
+  <si>
+    <t>s-400</t>
+  </si>
+  <si>
+    <t>c-220</t>
+  </si>
+  <si>
+    <t>lexus</t>
+  </si>
+  <si>
+    <t>rc-300</t>
+  </si>
+  <si>
+    <t>nx-300h</t>
+  </si>
+  <si>
+    <t>jeep</t>
+  </si>
+  <si>
+    <t>cherokee</t>
+  </si>
+  <si>
+    <t>jaguar</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>grace</t>
+  </si>
+  <si>
+    <t>holden</t>
+  </si>
+  <si>
+    <t>colorado</t>
+  </si>
+  <si>
+    <t>m235i</t>
+  </si>
+  <si>
+    <t>435i</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>harrier</t>
+  </si>
+  <si>
+    <t>cx-9</t>
+  </si>
+  <si>
+    <t>vezel</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>sq5</t>
+  </si>
+  <si>
+    <t>rvr</t>
+  </si>
+  <si>
+    <t>cla-45</t>
+  </si>
+  <si>
+    <t>a-180</t>
+  </si>
+  <si>
+    <t>cx-5</t>
   </si>
   <si>
     <t>range-rover-evoque</t>
   </si>
   <si>
-    <t>kia</t>
-  </si>
-  <si>
-    <t>sorento</t>
-  </si>
-  <si>
-    <t>niro</t>
-  </si>
-  <si>
-    <t>isuzu</t>
-  </si>
-  <si>
-    <t>mu-x</t>
-  </si>
-  <si>
-    <t>d-max</t>
-  </si>
-  <si>
-    <t>hyundai</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>tucson</t>
-  </si>
-  <si>
-    <t>santa-fe</t>
-  </si>
-  <si>
-    <t>palisade</t>
-  </si>
-  <si>
-    <t>kona</t>
-  </si>
-  <si>
-    <t>ioniq</t>
-  </si>
-  <si>
-    <t>i30-n</t>
-  </si>
-  <si>
-    <t>i30</t>
-  </si>
-  <si>
-    <t>i20</t>
-  </si>
-  <si>
-    <t>ford</t>
-  </si>
-  <si>
-    <t>transit</t>
-  </si>
-  <si>
-    <t>puma</t>
-  </si>
-  <si>
-    <t>escape</t>
-  </si>
-  <si>
-    <t>citroen</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>byd</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>bmw</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
-    <t>alfa-romeo</t>
-  </si>
-  <si>
-    <t>stelvio</t>
-  </si>
-  <si>
-    <t>t-roc</t>
-  </si>
-  <si>
-    <t>yaris</t>
-  </si>
-  <si>
-    <t>land-cruiser</t>
-  </si>
-  <si>
-    <t>highlander</t>
-  </si>
-  <si>
-    <t>mercedes-benz</t>
-  </si>
-  <si>
-    <t>e-300</t>
-  </si>
-  <si>
-    <t>staria</t>
-  </si>
-  <si>
-    <t>530e</t>
-  </si>
-  <si>
-    <t>supra</t>
-  </si>
-  <si>
-    <t>rav4</t>
-  </si>
-  <si>
-    <t>raize</t>
-  </si>
-  <si>
-    <t>hilux</t>
-  </si>
-  <si>
-    <t>porsche</t>
-  </si>
-  <si>
-    <t>cayenne</t>
-  </si>
-  <si>
-    <t>nissan</t>
-  </si>
-  <si>
-    <t>leaf</t>
-  </si>
-  <si>
-    <t>juke</t>
-  </si>
-  <si>
-    <t>honda</t>
-  </si>
-  <si>
-    <t>hr-v</t>
-  </si>
-  <si>
-    <t>v60</t>
-  </si>
-  <si>
-    <t>fortuner</t>
-  </si>
-  <si>
-    <t>corolla</t>
-  </si>
-  <si>
-    <t>camry</t>
-  </si>
-  <si>
-    <t>panamera</t>
-  </si>
-  <si>
-    <t>nv350</t>
-  </si>
-  <si>
-    <t>mazda</t>
-  </si>
-  <si>
-    <t>cx-30</t>
-  </si>
-  <si>
-    <t>range-rover-sport</t>
-  </si>
-  <si>
-    <t>seltos</t>
-  </si>
-  <si>
-    <t>accent</t>
-  </si>
-  <si>
-    <t>ranger</t>
-  </si>
-  <si>
-    <t>endura</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>740e</t>
-  </si>
-  <si>
-    <t>golf</t>
-  </si>
-  <si>
-    <t>hiace</t>
-  </si>
-  <si>
-    <t>c-hr</t>
-  </si>
-  <si>
-    <t>aqua</t>
-  </si>
-  <si>
-    <t>mini</t>
-  </si>
-  <si>
-    <t>countryman</t>
-  </si>
-  <si>
-    <t>cooper</t>
-  </si>
-  <si>
-    <t>e-350</t>
-  </si>
-  <si>
-    <t>discovery-sport</t>
-  </si>
-  <si>
-    <t>holden</t>
-  </si>
-  <si>
-    <t>captiva</t>
-  </si>
-  <si>
-    <t>audi</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>tiguan</t>
-  </si>
-  <si>
-    <t>vitz</t>
-  </si>
-  <si>
-    <t>subaru</t>
-  </si>
-  <si>
-    <t>xv</t>
-  </si>
-  <si>
-    <t>forester</t>
-  </si>
-  <si>
-    <t>c-350-e</t>
-  </si>
-  <si>
-    <t>cx-3</t>
-  </si>
-  <si>
-    <t>330e</t>
-  </si>
-  <si>
-    <t>polo</t>
-  </si>
-  <si>
-    <t>passat</t>
-  </si>
-  <si>
-    <t>land-cruiser-prado</t>
-  </si>
-  <si>
-    <t>sportage</t>
-  </si>
-  <si>
-    <t>225xe</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>jetta</t>
-  </si>
-  <si>
-    <t>macan</t>
-  </si>
-  <si>
-    <t>s-400</t>
-  </si>
-  <si>
-    <t>c-220</t>
-  </si>
-  <si>
-    <t>lexus</t>
-  </si>
-  <si>
-    <t>rc-300</t>
-  </si>
-  <si>
-    <t>nx-300h</t>
-  </si>
-  <si>
-    <t>jaguar</t>
-  </si>
-  <si>
-    <t>xf</t>
-  </si>
-  <si>
-    <t>grace</t>
-  </si>
-  <si>
-    <t>colorado</t>
-  </si>
-  <si>
-    <t>m235i</t>
-  </si>
-  <si>
-    <t>i8</t>
-  </si>
-  <si>
-    <t>435i</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>harrier</t>
-  </si>
-  <si>
-    <t>cx-9</t>
-  </si>
-  <si>
-    <t>vezel</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>sq5</t>
-  </si>
-  <si>
-    <t>rvr</t>
-  </si>
-  <si>
-    <t>cla-45</t>
-  </si>
-  <si>
-    <t>a-180</t>
-  </si>
-  <si>
-    <t>cx-5</t>
-  </si>
-  <si>
     <t>commodore</t>
   </si>
   <si>
@@ -509,9 +500,6 @@
     <t>gs-250</t>
   </si>
   <si>
-    <t>range-rover</t>
-  </si>
-  <si>
     <t>116i</t>
   </si>
   <si>
@@ -527,9 +515,6 @@
     <t>x-trail</t>
   </si>
   <si>
-    <t>getz</t>
-  </si>
-  <si>
     <t>320i</t>
   </si>
   <si>
@@ -543,6 +528,9 @@
   </si>
   <si>
     <t>slk-350</t>
+  </si>
+  <si>
+    <t>300-e</t>
   </si>
 </sst>
 </file>
@@ -893,8 +881,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610AEF75-CCED-45D4-92E4-B5C558A07A8F}">
-  <dimension ref="A1:D258"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A512A2-3844-49BF-AAEF-AD54F5979468}">
+  <dimension ref="A1:D246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -967,7 +955,7 @@
         <v>2022</v>
       </c>
       <c r="D5">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1023,7 +1011,7 @@
         <v>2022</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1037,7 +1025,7 @@
         <v>2022</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1051,7 +1039,7 @@
         <v>2022</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1177,7 +1165,7 @@
         <v>2022</v>
       </c>
       <c r="D20">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1205,7 +1193,7 @@
         <v>2022</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1219,7 +1207,7 @@
         <v>2022</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1261,7 +1249,7 @@
         <v>2022</v>
       </c>
       <c r="D26">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1289,7 +1277,7 @@
         <v>2022</v>
       </c>
       <c r="D28">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1303,7 +1291,7 @@
         <v>2022</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1317,7 +1305,7 @@
         <v>2022</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1331,7 +1319,7 @@
         <v>2022</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1345,7 +1333,7 @@
         <v>2022</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1359,26 +1347,26 @@
         <v>2022</v>
       </c>
       <c r="D33">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>2022</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
@@ -1387,12 +1375,12 @@
         <v>2022</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
@@ -1401,12 +1389,12 @@
         <v>2022</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -1420,7 +1408,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
@@ -1429,7 +1417,7 @@
         <v>2022</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1443,60 +1431,60 @@
         <v>2022</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40">
         <v>2022</v>
       </c>
       <c r="D40">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C41">
         <v>2022</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C42">
         <v>2022</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1504,27 +1492,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C44">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>60</v>
       </c>
       <c r="C45">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -1532,24 +1520,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C47">
         <v>2021</v>
@@ -1560,10 +1548,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48">
         <v>2021</v>
@@ -1574,80 +1562,80 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C49">
         <v>2021</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="B50">
+        <v>508</v>
       </c>
       <c r="C50">
         <v>2021</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>2021</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C52">
         <v>2021</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C53">
         <v>2021</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54">
-        <v>508</v>
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
       </c>
       <c r="C54">
         <v>2021</v>
@@ -1658,38 +1646,38 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C55">
         <v>2021</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C56">
         <v>2021</v>
       </c>
       <c r="D56">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1700,10 +1688,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1714,66 +1702,66 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>2021</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C60">
         <v>2021</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C61">
         <v>2021</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C62">
         <v>2021</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1784,13 +1772,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C64">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -1798,13 +1786,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C65">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1812,13 +1800,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C66">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -1826,13 +1814,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C67">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -1840,24 +1828,24 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C68">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="B69">
+        <v>2008</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1868,10 +1856,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C70">
         <v>2020</v>
@@ -1882,24 +1870,24 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C71">
         <v>2020</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C72">
         <v>2020</v>
@@ -1910,38 +1898,38 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C73">
         <v>2020</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C74">
         <v>2020</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>22</v>
-      </c>
-      <c r="B75">
-        <v>2008</v>
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
       </c>
       <c r="C75">
         <v>2020</v>
@@ -1952,10 +1940,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>58</v>
-      </c>
-      <c r="B76" t="s">
-        <v>58</v>
+        <v>30</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -1966,16 +1954,16 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C77">
         <v>2020</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -1983,7 +1971,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C78">
         <v>2020</v>
@@ -1994,41 +1982,41 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C79">
         <v>2020</v>
       </c>
       <c r="D79">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80">
+        <v>2019</v>
+      </c>
+      <c r="D80">
         <v>4</v>
-      </c>
-      <c r="B80" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80">
-        <v>2020</v>
-      </c>
-      <c r="D80">
-        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>30</v>
-      </c>
-      <c r="B81">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
       </c>
       <c r="C81">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -2036,41 +2024,41 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C82">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C83">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C84">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2078,13 +2066,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="B85" t="s">
         <v>81</v>
       </c>
       <c r="C85">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -2092,13 +2080,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C86">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -2106,10 +2094,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B87" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C87">
         <v>2019</v>
@@ -2120,52 +2108,52 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C88">
         <v>2019</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>2019</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="C90">
         <v>2019</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="C91">
         <v>2019</v>
@@ -2176,7 +2164,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
         <v>85</v>
@@ -2190,10 +2178,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>18</v>
-      </c>
-      <c r="B93" t="s">
-        <v>20</v>
+        <v>84</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
       </c>
       <c r="C93">
         <v>2019</v>
@@ -2204,7 +2192,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="B94" t="s">
         <v>86</v>
@@ -2218,10 +2206,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C95">
         <v>2019</v>
@@ -2232,10 +2220,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="C96">
         <v>2019</v>
@@ -2246,38 +2234,38 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="C97">
         <v>2019</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C98">
         <v>2019</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B99" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C99">
         <v>2019</v>
@@ -2288,10 +2276,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C100">
         <v>2019</v>
@@ -2302,24 +2290,24 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>88</v>
-      </c>
-      <c r="B101">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="B101" t="s">
+        <v>91</v>
       </c>
       <c r="C101">
         <v>2019</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C102">
         <v>2019</v>
@@ -2330,13 +2318,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C103">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -2344,27 +2332,27 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C104">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C105">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -2372,55 +2360,55 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C106">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D106">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C107">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C108">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C109">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -2428,150 +2416,150 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C110">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C111">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C112">
         <v>2018</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="C113">
         <v>2018</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B114" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C114">
         <v>2018</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>2018</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C116">
         <v>2018</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="C117">
         <v>2018</v>
       </c>
       <c r="D117">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B118" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C118">
         <v>2018</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B119" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C119">
         <v>2018</v>
       </c>
       <c r="D119">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C120">
         <v>2018</v>
@@ -2582,66 +2570,66 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C121">
         <v>2018</v>
       </c>
       <c r="D121">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B122" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C122">
         <v>2018</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B123" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="C123">
         <v>2018</v>
       </c>
       <c r="D123">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="C124">
         <v>2018</v>
       </c>
       <c r="D124">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="B125" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C125">
         <v>2018</v>
@@ -2652,13 +2640,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C126">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -2666,55 +2654,55 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="C127">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C128">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C129">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="C130">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -2722,13 +2710,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C131">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -2736,13 +2724,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C132">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -2750,41 +2738,41 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C133">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="B134" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C134">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D134">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>106</v>
+      </c>
+      <c r="B135" t="s">
         <v>108</v>
       </c>
-      <c r="B135" t="s">
-        <v>109</v>
-      </c>
       <c r="C135">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -2792,10 +2780,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B136" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C136">
         <v>2017</v>
@@ -2806,91 +2794,91 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B137" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C137">
         <v>2017</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B138" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C138">
         <v>2017</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C139">
         <v>2017</v>
       </c>
       <c r="D139">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="C140">
         <v>2017</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C141">
         <v>2017</v>
       </c>
       <c r="D141">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C142">
         <v>2017</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B143" t="s">
         <v>99</v>
@@ -2899,29 +2887,29 @@
         <v>2017</v>
       </c>
       <c r="D143">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B144" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C144">
         <v>2017</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C145">
         <v>2017</v>
@@ -2932,139 +2920,139 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B146" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C146">
         <v>2017</v>
       </c>
       <c r="D146">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B147" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C147">
         <v>2017</v>
       </c>
       <c r="D147">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B148" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C148">
         <v>2017</v>
       </c>
       <c r="D148">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C149">
         <v>2017</v>
       </c>
       <c r="D149">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B150" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="C150">
         <v>2017</v>
       </c>
       <c r="D150">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C151">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D151">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C152">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C153">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B154" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C154">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D154">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="B155" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C155">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -3072,125 +3060,125 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B156" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C156">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D156">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B157" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C157">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D157">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B158" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C158">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B159" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C159">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D159">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C160">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D160">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B161" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C161">
         <v>2016</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B162" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C162">
         <v>2016</v>
       </c>
       <c r="D162">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B163" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C163">
         <v>2016</v>
       </c>
       <c r="D163">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B164" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="C164">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -3198,55 +3186,55 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B165" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C165">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C166">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D166">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B167" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C167">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D167">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B168" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C168">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -3254,69 +3242,69 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C169">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D169">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B170" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C170">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D170">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B171" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C171">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D171">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="B172" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="C172">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D172">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B173" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C173">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -3324,10 +3312,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B174" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C174">
         <v>2015</v>
@@ -3338,38 +3326,38 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="B175" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C175">
         <v>2015</v>
       </c>
       <c r="D175">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="B176" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="C176">
         <v>2015</v>
       </c>
       <c r="D176">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="B177" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C177">
         <v>2015</v>
@@ -3380,10 +3368,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B178" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C178">
         <v>2015</v>
@@ -3394,10 +3382,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B179" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C179">
         <v>2015</v>
@@ -3408,24 +3396,24 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>133</v>
       </c>
       <c r="C180">
         <v>2015</v>
       </c>
       <c r="D180">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B181" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C181">
         <v>2015</v>
@@ -3436,10 +3424,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B182" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C182">
         <v>2015</v>
@@ -3450,10 +3438,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B183" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="C183">
         <v>2015</v>
@@ -3464,13 +3452,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="B184" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C184">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D184">
         <v>1</v>
@@ -3478,27 +3466,27 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="B185" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="C185">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D185">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="B186" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="C186">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -3506,13 +3494,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B187" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C187">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D187">
         <v>1</v>
@@ -3520,13 +3508,13 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B188" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="C188">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D188">
         <v>1</v>
@@ -3534,27 +3522,27 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C189">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D189">
-        <v>1</v>
+        <v>113</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C190">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -3562,13 +3550,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="B191" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C191">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -3576,27 +3564,27 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B192" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C192">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="B193" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
       <c r="C193">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -3604,13 +3592,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B194" t="s">
         <v>139</v>
       </c>
       <c r="C194">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -3618,44 +3606,44 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B195" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C195">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D195">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B196" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C196">
         <v>2014</v>
       </c>
       <c r="D196">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B197" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C197">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D197">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
@@ -3663,10 +3651,10 @@
         <v>11</v>
       </c>
       <c r="B198" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C198">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D198">
         <v>1</v>
@@ -3677,52 +3665,52 @@
         <v>11</v>
       </c>
       <c r="B199" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="C199">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D199">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B200" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="C200">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D200">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B201" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C201">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D201">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="B202" t="s">
         <v>141</v>
       </c>
       <c r="C202">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D202">
         <v>1</v>
@@ -3730,41 +3718,41 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="C203">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D203">
-        <v>1</v>
+        <v>161</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B204" t="s">
         <v>142</v>
       </c>
       <c r="C204">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D204">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="B205" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="C205">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D205">
         <v>1</v>
@@ -3772,27 +3760,27 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B206" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C206">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D206">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="B207" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="C207">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D207">
         <v>1</v>
@@ -3800,38 +3788,38 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="B208" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C208">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D208">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B209" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="C209">
         <v>2013</v>
       </c>
       <c r="D209">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="B210" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="C210">
         <v>2013</v>
@@ -3842,27 +3830,27 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B211" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C211">
         <v>2013</v>
       </c>
       <c r="D211">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="B212" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C212">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D212">
         <v>2</v>
@@ -3870,13 +3858,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B213" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="C213">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D213">
         <v>1</v>
@@ -3884,41 +3872,41 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B214" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="C214">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D214">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B215" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="C215">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D215">
-        <v>163</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="B216" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
       <c r="C216">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -3926,41 +3914,41 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>147</v>
+        <v>25</v>
       </c>
       <c r="C217">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D217">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="B218" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C218">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D218">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B219" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="C219">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -3968,13 +3956,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B220" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="C220">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -3982,66 +3970,66 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B221" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="C221">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D221">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B222" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C222">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D222">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="B223" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="C223">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D223">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B224" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="C224">
         <v>2012</v>
       </c>
       <c r="D224">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B225" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C225">
         <v>2012</v>
@@ -4052,38 +4040,38 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="B226" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="C226">
         <v>2012</v>
       </c>
       <c r="D226">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B227" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="C227">
         <v>2012</v>
       </c>
       <c r="D227">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B228" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C228">
         <v>2012</v>
@@ -4094,24 +4082,24 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B229" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="C229">
         <v>2012</v>
       </c>
       <c r="D229">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B230" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C230">
         <v>2012</v>
@@ -4122,13 +4110,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B231" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="C231">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D231">
         <v>1</v>
@@ -4136,13 +4124,13 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B232" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="C232">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D232">
         <v>1</v>
@@ -4150,13 +4138,13 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B233" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C233">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D233">
         <v>1</v>
@@ -4164,16 +4152,16 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B234" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C234">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D234">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
@@ -4181,38 +4169,38 @@
         <v>128</v>
       </c>
       <c r="B235" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="C235">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D235">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B236" t="s">
         <v>156</v>
       </c>
       <c r="C236">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D236">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B237" t="s">
         <v>157</v>
       </c>
       <c r="C237">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D237">
         <v>1</v>
@@ -4220,13 +4208,13 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="B238" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="C238">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D238">
         <v>1</v>
@@ -4234,13 +4222,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B239" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="C239">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D239">
         <v>1</v>
@@ -4248,13 +4236,13 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="B240" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="C240">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="D240">
         <v>1</v>
@@ -4262,13 +4250,13 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="B241" t="s">
-        <v>143</v>
+        <v>23</v>
       </c>
       <c r="C241">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="D241">
         <v>1</v>
@@ -4276,13 +4264,13 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B242" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C242">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="D242">
         <v>1</v>
@@ -4290,13 +4278,13 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B243" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="C243">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="D243">
         <v>1</v>
@@ -4304,13 +4292,13 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="B244" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="C244">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="D244">
         <v>1</v>
@@ -4318,13 +4306,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="B245" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="C245">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="D245">
         <v>1</v>
@@ -4332,183 +4320,15 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>128</v>
+        <v>63</v>
       </c>
       <c r="B246" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C246">
-        <v>2011</v>
+        <v>1991</v>
       </c>
       <c r="D246">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>131</v>
-      </c>
-      <c r="B247" t="s">
-        <v>132</v>
-      </c>
-      <c r="C247">
-        <v>2011</v>
-      </c>
-      <c r="D247">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>80</v>
-      </c>
-      <c r="B248" t="s">
-        <v>160</v>
-      </c>
-      <c r="C248">
-        <v>2011</v>
-      </c>
-      <c r="D248">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>59</v>
-      </c>
-      <c r="B249" t="s">
-        <v>161</v>
-      </c>
-      <c r="C249">
-        <v>2011</v>
-      </c>
-      <c r="D249">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>77</v>
-      </c>
-      <c r="B250" t="s">
-        <v>162</v>
-      </c>
-      <c r="C250">
-        <v>2009</v>
-      </c>
-      <c r="D250">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>41</v>
-      </c>
-      <c r="B251" t="s">
-        <v>163</v>
-      </c>
-      <c r="C251">
-        <v>2009</v>
-      </c>
-      <c r="D251">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>59</v>
-      </c>
-      <c r="B252" t="s">
-        <v>164</v>
-      </c>
-      <c r="C252">
-        <v>2009</v>
-      </c>
-      <c r="D252">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>165</v>
-      </c>
-      <c r="B253" t="s">
-        <v>166</v>
-      </c>
-      <c r="C253">
-        <v>2007</v>
-      </c>
-      <c r="D253">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>166</v>
-      </c>
-      <c r="B254" t="s">
-        <v>23</v>
-      </c>
-      <c r="C254">
-        <v>2007</v>
-      </c>
-      <c r="D254">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>59</v>
-      </c>
-      <c r="B255" t="s">
-        <v>167</v>
-      </c>
-      <c r="C255">
-        <v>2006</v>
-      </c>
-      <c r="D255">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>11</v>
-      </c>
-      <c r="B256" t="s">
-        <v>65</v>
-      </c>
-      <c r="C256">
-        <v>2005</v>
-      </c>
-      <c r="D256">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>67</v>
-      </c>
-      <c r="B257" t="s">
-        <v>168</v>
-      </c>
-      <c r="C257">
-        <v>2005</v>
-      </c>
-      <c r="D257">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>11</v>
-      </c>
-      <c r="B258" t="s">
-        <v>12</v>
-      </c>
-      <c r="C258">
-        <v>2004</v>
-      </c>
-      <c r="D258">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update and merge with kirsty's changes
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somet\Documents\Engineering\PartIV\762\762-impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiaru\Documents\UiPath\762-impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6167890-5C28-4793-9576-DC5A2EBADA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D275A6-E329-4561-AAD4-F34A4E2DFF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="2400" windowWidth="32505" windowHeight="15345" xr2:uid="{4A9C7B27-1D65-4421-A46B-644C7F91AB91}"/>
+    <workbookView xWindow="1635" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{4A75A796-F6A9-442D-AA11-4067559B62C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="159">
   <si>
     <t>Make</t>
   </si>
@@ -59,6 +57,9 @@
     <t>volvo</t>
   </si>
   <si>
+    <t>xc90</t>
+  </si>
+  <si>
     <t>xc60</t>
   </si>
   <si>
@@ -68,189 +69,189 @@
     <t>multivan</t>
   </si>
   <si>
+    <t>tesla</t>
+  </si>
+  <si>
+    <t>model-y</t>
+  </si>
+  <si>
+    <t>skoda</t>
+  </si>
+  <si>
+    <t>superb</t>
+  </si>
+  <si>
+    <t>octavia</t>
+  </si>
+  <si>
+    <t>renault</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>koleos</t>
+  </si>
+  <si>
+    <t>kadjar</t>
+  </si>
+  <si>
+    <t>arkana</t>
+  </si>
+  <si>
+    <t>peugeot</t>
+  </si>
+  <si>
+    <t>triton</t>
+  </si>
+  <si>
+    <t>pajero</t>
+  </si>
+  <si>
+    <t>mirage</t>
+  </si>
+  <si>
+    <t>express</t>
+  </si>
+  <si>
+    <t>eclipse-cross</t>
+  </si>
+  <si>
+    <t>asx</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>land-rover</t>
+  </si>
+  <si>
+    <t>range-rover-velar</t>
+  </si>
+  <si>
+    <t>range-rover-evoque</t>
+  </si>
+  <si>
+    <t>range-rover</t>
+  </si>
+  <si>
+    <t>kia</t>
+  </si>
+  <si>
+    <t>sorento</t>
+  </si>
+  <si>
+    <t>niro</t>
+  </si>
+  <si>
+    <t>isuzu</t>
+  </si>
+  <si>
+    <t>mu-x</t>
+  </si>
+  <si>
+    <t>d-max</t>
+  </si>
+  <si>
+    <t>hyundai</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>santa-fe</t>
+  </si>
+  <si>
+    <t>kona</t>
+  </si>
+  <si>
+    <t>ioniq-5</t>
+  </si>
+  <si>
+    <t>ioniq</t>
+  </si>
+  <si>
+    <t>i30-n</t>
+  </si>
+  <si>
+    <t>i30</t>
+  </si>
+  <si>
+    <t>i20</t>
+  </si>
+  <si>
+    <t>ford</t>
+  </si>
+  <si>
+    <t>transit</t>
+  </si>
+  <si>
+    <t>puma</t>
+  </si>
+  <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>citroen</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>byd</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>alfa-romeo</t>
+  </si>
+  <si>
+    <t>stelvio</t>
+  </si>
+  <si>
+    <t>t-roc</t>
+  </si>
+  <si>
     <t>toyota</t>
   </si>
   <si>
-    <t>land-cruiser</t>
+    <t>yaris</t>
+  </si>
+  <si>
+    <t>rav4</t>
+  </si>
+  <si>
+    <t>prius</t>
+  </si>
+  <si>
+    <t>mercedes-benz</t>
+  </si>
+  <si>
+    <t>e-300</t>
+  </si>
+  <si>
+    <t>staria</t>
+  </si>
+  <si>
+    <t>supra</t>
+  </si>
+  <si>
+    <t>raize</t>
   </si>
   <si>
     <t>hilux</t>
   </si>
   <si>
-    <t>tesla</t>
-  </si>
-  <si>
-    <t>model-y</t>
-  </si>
-  <si>
-    <t>skoda</t>
-  </si>
-  <si>
-    <t>superb</t>
-  </si>
-  <si>
-    <t>octavia</t>
-  </si>
-  <si>
-    <t>renault</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t>koleos</t>
-  </si>
-  <si>
-    <t>kadjar</t>
-  </si>
-  <si>
-    <t>arkana</t>
-  </si>
-  <si>
-    <t>peugeot</t>
-  </si>
-  <si>
-    <t>listing</t>
-  </si>
-  <si>
-    <t>triton</t>
-  </si>
-  <si>
-    <t>pajero</t>
-  </si>
-  <si>
-    <t>mirage</t>
-  </si>
-  <si>
-    <t>express</t>
-  </si>
-  <si>
-    <t>eclipse-cross</t>
-  </si>
-  <si>
-    <t>asx</t>
-  </si>
-  <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>hs</t>
-  </si>
-  <si>
-    <t>land-rover</t>
-  </si>
-  <si>
-    <t>range-rover-velar</t>
-  </si>
-  <si>
-    <t>range-rover-evoque</t>
-  </si>
-  <si>
-    <t>range-rover</t>
-  </si>
-  <si>
-    <t>kia</t>
-  </si>
-  <si>
-    <t>sorento</t>
-  </si>
-  <si>
-    <t>niro</t>
-  </si>
-  <si>
-    <t>isuzu</t>
-  </si>
-  <si>
-    <t>mu-x</t>
-  </si>
-  <si>
-    <t>d-max</t>
-  </si>
-  <si>
-    <t>hyundai</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>santa-fe</t>
-  </si>
-  <si>
-    <t>kona</t>
-  </si>
-  <si>
-    <t>ioniq-5</t>
-  </si>
-  <si>
-    <t>ioniq</t>
-  </si>
-  <si>
-    <t>i30-n</t>
-  </si>
-  <si>
-    <t>i30</t>
-  </si>
-  <si>
-    <t>i20</t>
-  </si>
-  <si>
-    <t>ford</t>
-  </si>
-  <si>
-    <t>transit</t>
-  </si>
-  <si>
-    <t>puma</t>
-  </si>
-  <si>
-    <t>escape</t>
-  </si>
-  <si>
-    <t>citroen</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>byd</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>bmw</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
-    <t>alfa-romeo</t>
-  </si>
-  <si>
-    <t>stelvio</t>
-  </si>
-  <si>
-    <t>t-roc</t>
-  </si>
-  <si>
-    <t>yaris</t>
-  </si>
-  <si>
-    <t>prius</t>
-  </si>
-  <si>
-    <t>mercedes-benz</t>
-  </si>
-  <si>
-    <t>e-300</t>
-  </si>
-  <si>
-    <t>staria</t>
-  </si>
-  <si>
-    <t>supra</t>
-  </si>
-  <si>
     <t>suzuki</t>
   </si>
   <si>
@@ -266,238 +267,232 @@
     <t>juke</t>
   </si>
   <si>
+    <t>530e</t>
+  </si>
+  <si>
+    <t>v60</t>
+  </si>
+  <si>
+    <t>fortuner</t>
+  </si>
+  <si>
+    <t>corolla</t>
+  </si>
+  <si>
+    <t>camry</t>
+  </si>
+  <si>
+    <t>porsche</t>
+  </si>
+  <si>
+    <t>panamera</t>
+  </si>
+  <si>
+    <t>cayenne</t>
+  </si>
+  <si>
+    <t>nv350</t>
+  </si>
+  <si>
+    <t>mazda</t>
+  </si>
+  <si>
+    <t>cx-30</t>
+  </si>
+  <si>
+    <t>range-rover-sport</t>
+  </si>
+  <si>
+    <t>tucson</t>
+  </si>
+  <si>
+    <t>accent</t>
+  </si>
+  <si>
+    <t>740e</t>
+  </si>
+  <si>
+    <t>golf</t>
+  </si>
+  <si>
+    <t>highlander</t>
+  </si>
+  <si>
+    <t>hiace</t>
+  </si>
+  <si>
+    <t>c-hr</t>
+  </si>
+  <si>
+    <t>aqua</t>
+  </si>
+  <si>
+    <t>mini</t>
+  </si>
+  <si>
+    <t>countryman</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>e-350</t>
+  </si>
+  <si>
+    <t>tiguan</t>
+  </si>
+  <si>
+    <t>vitz</t>
+  </si>
+  <si>
+    <t>subaru</t>
+  </si>
+  <si>
+    <t>xv</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>c-350-e</t>
+  </si>
+  <si>
+    <t>territory</t>
+  </si>
+  <si>
+    <t>330e</t>
+  </si>
+  <si>
+    <t>225xe</t>
+  </si>
+  <si>
+    <t>polo</t>
+  </si>
+  <si>
+    <t>passat</t>
+  </si>
+  <si>
+    <t>audi</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>jetta</t>
+  </si>
+  <si>
+    <t>macan</t>
+  </si>
+  <si>
+    <t>e-nv200</t>
+  </si>
+  <si>
+    <t>s-400</t>
+  </si>
+  <si>
+    <t>c-250</t>
+  </si>
+  <si>
+    <t>c-220</t>
+  </si>
+  <si>
+    <t>lexus</t>
+  </si>
+  <si>
+    <t>rc-300</t>
+  </si>
+  <si>
+    <t>jaguar</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>holden</t>
+  </si>
+  <si>
+    <t>colorado</t>
+  </si>
+  <si>
+    <t>m235i</t>
+  </si>
+  <si>
+    <t>i8</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>harrier</t>
+  </si>
+  <si>
+    <t>cx-9</t>
+  </si>
+  <si>
+    <t>nx-300h</t>
+  </si>
+  <si>
     <t>honda</t>
   </si>
   <si>
-    <t>hr-v</t>
-  </si>
-  <si>
-    <t>530e</t>
-  </si>
-  <si>
-    <t>v60</t>
-  </si>
-  <si>
-    <t>rav4</t>
-  </si>
-  <si>
-    <t>fortuner</t>
-  </si>
-  <si>
-    <t>corolla</t>
-  </si>
-  <si>
-    <t>camry</t>
-  </si>
-  <si>
-    <t>porsche</t>
-  </si>
-  <si>
-    <t>panamera</t>
-  </si>
-  <si>
-    <t>cayenne</t>
-  </si>
-  <si>
-    <t>nv350</t>
-  </si>
-  <si>
-    <t>mazda</t>
-  </si>
-  <si>
-    <t>cx-30</t>
-  </si>
-  <si>
-    <t>range-rover-sport</t>
-  </si>
-  <si>
-    <t>seltos</t>
-  </si>
-  <si>
-    <t>tucson</t>
-  </si>
-  <si>
-    <t>accent</t>
-  </si>
-  <si>
-    <t>740e</t>
-  </si>
-  <si>
-    <t>golf</t>
-  </si>
-  <si>
-    <t>highlander</t>
-  </si>
-  <si>
-    <t>hiace</t>
-  </si>
-  <si>
-    <t>c-hr</t>
-  </si>
-  <si>
-    <t>aqua</t>
-  </si>
-  <si>
-    <t>mini</t>
-  </si>
-  <si>
-    <t>countryman</t>
-  </si>
-  <si>
-    <t>cooper</t>
-  </si>
-  <si>
-    <t>e-350</t>
-  </si>
-  <si>
-    <t>tiguan</t>
-  </si>
-  <si>
-    <t>vitz</t>
-  </si>
-  <si>
-    <t>subaru</t>
-  </si>
-  <si>
-    <t>xv</t>
-  </si>
-  <si>
-    <t>c-350-e</t>
-  </si>
-  <si>
-    <t>holden</t>
-  </si>
-  <si>
-    <t>astra</t>
-  </si>
-  <si>
-    <t>territory</t>
-  </si>
-  <si>
-    <t>330e</t>
-  </si>
-  <si>
-    <t>225xe</t>
-  </si>
-  <si>
-    <t>passat</t>
-  </si>
-  <si>
-    <t>land-cruiser-prado</t>
-  </si>
-  <si>
-    <t>audi</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>jetta</t>
-  </si>
-  <si>
-    <t>outback</t>
-  </si>
-  <si>
-    <t>macan</t>
-  </si>
-  <si>
-    <t>e-nv200</t>
-  </si>
-  <si>
-    <t>s-400</t>
-  </si>
-  <si>
-    <t>c-250</t>
-  </si>
-  <si>
-    <t>c-220</t>
-  </si>
-  <si>
-    <t>lexus</t>
-  </si>
-  <si>
-    <t>rc-300</t>
-  </si>
-  <si>
-    <t>nx-300h</t>
-  </si>
-  <si>
-    <t>jaguar</t>
-  </si>
-  <si>
-    <t>xf</t>
-  </si>
-  <si>
-    <t>grace</t>
-  </si>
-  <si>
-    <t>colorado</t>
-  </si>
-  <si>
-    <t>i8</t>
-  </si>
-  <si>
-    <t>435i</t>
-  </si>
-  <si>
-    <t>harrier</t>
-  </si>
-  <si>
-    <t>cx-9</t>
-  </si>
-  <si>
     <t>vezel</t>
   </si>
   <si>
+    <t>sq5</t>
+  </si>
+  <si>
+    <t>navara</t>
+  </si>
+  <si>
+    <t>rvr</t>
+  </si>
+  <si>
+    <t>cla-45</t>
+  </si>
+  <si>
+    <t>a-180</t>
+  </si>
+  <si>
+    <t>cx-5</t>
+  </si>
+  <si>
+    <t>commodore</t>
+  </si>
+  <si>
+    <t>lancer</t>
+  </si>
+  <si>
+    <t>r-350</t>
+  </si>
+  <si>
+    <t>ml-350</t>
+  </si>
+  <si>
+    <t>c-180</t>
+  </si>
+  <si>
+    <t>rx-450h</t>
+  </si>
+  <si>
+    <t>ls-600</t>
+  </si>
+  <si>
+    <t>gs-250</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
     <t>116i</t>
   </si>
   <si>
-    <t>sq5</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>rvr</t>
-  </si>
-  <si>
-    <t>cla-45</t>
-  </si>
-  <si>
-    <t>cx-5</t>
-  </si>
-  <si>
-    <t>commodore</t>
-  </si>
-  <si>
-    <t>lancer</t>
-  </si>
-  <si>
-    <t>ml-350</t>
-  </si>
-  <si>
-    <t>rx-450h</t>
-  </si>
-  <si>
-    <t>ls-600</t>
-  </si>
-  <si>
-    <t>gs-250</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>328i</t>
-  </si>
-  <si>
-    <t>polo</t>
-  </si>
-  <si>
     <t>fit</t>
   </si>
   <si>
     <t>kuga</t>
+  </si>
+  <si>
+    <t>523i</t>
   </si>
   <si>
     <t>x-trail</t>
@@ -866,8 +861,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9075A47D-84DE-4F8C-8476-FA06FE2480B8}">
-  <dimension ref="A1:D236"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C06B43-F583-4687-B11F-98B0E0DF934B}">
+  <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -912,40 +907,40 @@
         <v>2022</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>2022</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5">
         <v>2022</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -968,15 +963,15 @@
         <v>2022</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8">
         <v>2022</v>
@@ -987,7 +982,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1001,24 +996,24 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
       <c r="C10">
         <v>2022</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>2022</v>
@@ -1029,10 +1024,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>2022</v>
@@ -1043,44 +1038,44 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>3008</v>
       </c>
       <c r="C13">
         <v>2022</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>3008</v>
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2022</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>2022</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,13 +1083,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>2022</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1102,13 +1097,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>2022</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,13 +1111,13 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>2022</v>
       </c>
       <c r="D18">
-        <v>95</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,13 +1125,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>2022</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1144,18 +1139,18 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>2022</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -1164,26 +1159,26 @@
         <v>2022</v>
       </c>
       <c r="D21">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <v>2022</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -1192,15 +1187,15 @@
         <v>2022</v>
       </c>
       <c r="D23">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
         <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
       </c>
       <c r="C24">
         <v>2022</v>
@@ -1211,7 +1206,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
@@ -1220,12 +1215,12 @@
         <v>2022</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>36</v>
@@ -1234,7 +1229,7 @@
         <v>2022</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,7 +1243,7 @@
         <v>2022</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,7 +1257,7 @@
         <v>2022</v>
       </c>
       <c r="D28">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,7 +1271,7 @@
         <v>2022</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,57 +1285,57 @@
         <v>2022</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
         <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
       </c>
       <c r="C31">
         <v>2022</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>2022</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>2022</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>2022</v>
@@ -1351,24 +1346,24 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>2022</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>2022</v>
@@ -1379,7 +1374,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -1388,12 +1383,12 @@
         <v>2022</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
@@ -1402,88 +1397,88 @@
         <v>2022</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C39">
         <v>2022</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40">
         <v>2022</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C41">
         <v>2022</v>
       </c>
       <c r="D41">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C42">
         <v>2022</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <v>2022</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C44">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1491,30 +1486,30 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C45">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D45">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C46">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,21 +1517,21 @@
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C47">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>2021</v>
@@ -1547,10 +1542,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" t="s">
-        <v>64</v>
+        <v>21</v>
+      </c>
+      <c r="B49">
+        <v>508</v>
       </c>
       <c r="C49">
         <v>2021</v>
@@ -1561,10 +1556,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>2021</v>
@@ -1575,38 +1570,38 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C51">
         <v>2021</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C52">
         <v>2021</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -1617,66 +1612,66 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>23</v>
-      </c>
-      <c r="B54">
-        <v>508</v>
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>35</v>
       </c>
       <c r="C54">
         <v>2021</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C55">
         <v>2021</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C56">
         <v>2021</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C57">
         <v>2021</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1687,41 +1682,41 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C59">
         <v>2021</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C61">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -1729,27 +1724,27 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C62">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C63">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -1757,13 +1752,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C64">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -1771,24 +1766,24 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C65">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1799,38 +1794,38 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <v>2020</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C68">
         <v>2020</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1841,24 +1836,24 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" t="s">
-        <v>74</v>
+        <v>28</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
       </c>
       <c r="C70">
         <v>2020</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C71">
         <v>2020</v>
@@ -1869,41 +1864,41 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C72">
         <v>2020</v>
       </c>
       <c r="D72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C73">
         <v>2020</v>
       </c>
       <c r="D73">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C74">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -1911,27 +1906,27 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B75">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="B75" t="s">
+        <v>64</v>
       </c>
       <c r="C75">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C76">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -1939,52 +1934,52 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C77">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C79">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80">
         <v>2019</v>
@@ -1995,38 +1990,38 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C81">
         <v>2019</v>
       </c>
       <c r="D81">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>2019</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="C83">
         <v>2019</v>
@@ -2037,24 +2032,24 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C84">
         <v>2019</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C85">
         <v>2019</v>
@@ -2065,10 +2060,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="C86">
         <v>2019</v>
@@ -2079,10 +2074,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C87">
         <v>2019</v>
@@ -2093,24 +2088,24 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" t="s">
         <v>86</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
       </c>
       <c r="C88">
         <v>2019</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C89">
         <v>2019</v>
@@ -2121,10 +2116,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="C90">
         <v>2019</v>
@@ -2135,38 +2130,38 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C91">
         <v>2019</v>
       </c>
       <c r="D91">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B92" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C92">
         <v>2019</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B93" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C93">
         <v>2019</v>
@@ -2177,10 +2172,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C94">
         <v>2019</v>
@@ -2191,83 +2186,83 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>88</v>
-      </c>
-      <c r="B95">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>92</v>
       </c>
       <c r="C95">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C96">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C97">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B98" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="C98">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C99">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B100" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C100">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D100">
         <v>4</v>
@@ -2275,13 +2270,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B101" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C101">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -2289,24 +2284,24 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B102" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C102">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B103" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C103">
         <v>2018</v>
@@ -2317,38 +2312,38 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C104">
         <v>2018</v>
       </c>
       <c r="D104">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C105">
         <v>2018</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C106">
         <v>2018</v>
@@ -2359,24 +2354,24 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C107">
         <v>2018</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C108">
         <v>2018</v>
@@ -2387,10 +2382,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B109" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C109">
         <v>2018</v>
@@ -2401,24 +2396,24 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B110" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C110">
         <v>2018</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B111" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C111">
         <v>2018</v>
@@ -2429,10 +2424,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B112" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="C112">
         <v>2018</v>
@@ -2443,10 +2438,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C113">
         <v>2018</v>
@@ -2457,97 +2452,97 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="C114">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D114">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="C115">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D115">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B116" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="C116">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B117" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C117">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B118" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C118">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D118">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C119">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C120">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -2555,27 +2550,27 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B121" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="C121">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D121">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B122" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C122">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -2583,13 +2578,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B123" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C123">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -2597,24 +2592,24 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B124" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C124">
         <v>2017</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B125" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C125">
         <v>2017</v>
@@ -2625,94 +2620,94 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C126">
         <v>2017</v>
       </c>
       <c r="D126">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C127">
         <v>2017</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="C128">
         <v>2017</v>
       </c>
       <c r="D128">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C129">
         <v>2017</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="C130">
         <v>2017</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B131" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C131">
         <v>2017</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>73</v>
-      </c>
-      <c r="B132" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="B132">
+        <v>6</v>
       </c>
       <c r="C132">
         <v>2017</v>
@@ -2723,10 +2718,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B133" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="C133">
         <v>2017</v>
@@ -2737,97 +2732,97 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="C134">
         <v>2017</v>
       </c>
       <c r="D134">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B135" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C135">
         <v>2017</v>
       </c>
       <c r="D135">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B136" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C136">
         <v>2017</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B137" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C137">
         <v>2017</v>
       </c>
       <c r="D137">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B138" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C138">
         <v>2017</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B139" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C139">
         <v>2017</v>
       </c>
       <c r="D139">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>88</v>
-      </c>
-      <c r="B140">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>110</v>
       </c>
       <c r="C140">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -2835,13 +2830,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B141" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="C141">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D141">
         <v>3</v>
@@ -2849,27 +2844,27 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="B142" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C142">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B143" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="C143">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -2877,13 +2872,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B144" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C144">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D144">
         <v>2</v>
@@ -2891,13 +2886,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B145" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C145">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D145">
         <v>2</v>
@@ -2905,52 +2900,52 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C146">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D146">
-        <v>5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B147" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C147">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D147">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B148" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C148">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D148">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C149">
         <v>2016</v>
@@ -2961,69 +2956,69 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B150" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C150">
         <v>2016</v>
       </c>
       <c r="D150">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B151" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C151">
         <v>2016</v>
       </c>
       <c r="D151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="C152">
         <v>2016</v>
       </c>
       <c r="D152">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C153">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D153">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B154" t="s">
         <v>92</v>
       </c>
       <c r="C154">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D154">
         <v>3</v>
@@ -3031,55 +3026,55 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B155" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C155">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D155">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B156" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C156">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D156">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B157" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C157">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D157">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158" t="s">
         <v>116</v>
       </c>
-      <c r="B158" t="s">
-        <v>117</v>
-      </c>
       <c r="C158">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D158">
         <v>1</v>
@@ -3087,38 +3082,38 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B159" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="C159">
         <v>2015</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B160" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="C160">
         <v>2015</v>
       </c>
       <c r="D160">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B161" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C161">
         <v>2015</v>
@@ -3129,10 +3124,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B162" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="C162">
         <v>2015</v>
@@ -3143,10 +3138,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B163" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C163">
         <v>2015</v>
@@ -3157,10 +3152,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="B164" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C164">
         <v>2015</v>
@@ -3171,10 +3166,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B165" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="C165">
         <v>2015</v>
@@ -3185,24 +3180,24 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="C166">
         <v>2015</v>
       </c>
       <c r="D166">
-        <v>128</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B167" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="C167">
         <v>2015</v>
@@ -3213,10 +3208,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B168" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C168">
         <v>2015</v>
@@ -3227,10 +3222,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C169">
         <v>2015</v>
@@ -3241,10 +3236,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B170" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="C170">
         <v>2015</v>
@@ -3255,27 +3250,27 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B171" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C171">
         <v>2015</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="B172" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C172">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D172">
         <v>1</v>
@@ -3283,27 +3278,27 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="B173" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="C173">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D173">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B174" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C174">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D174">
         <v>1</v>
@@ -3311,27 +3306,27 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="C175">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D175">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B176" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C176">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D176">
         <v>1</v>
@@ -3339,13 +3334,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B177" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C177">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D177">
         <v>1</v>
@@ -3353,27 +3348,27 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="B178" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C178">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D178">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B179" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C179">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D179">
         <v>1</v>
@@ -3381,27 +3376,27 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B180" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C180">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D180">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B181" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C181">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -3409,27 +3404,27 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B182" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C182">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D182">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B183" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="C183">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -3437,41 +3432,41 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C184">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D184">
-        <v>116</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B185" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="C185">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D185">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="B186" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C186">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -3479,27 +3474,27 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B187" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C187">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D187">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="C188">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D188">
         <v>1</v>
@@ -3507,27 +3502,27 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="C189">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D189">
-        <v>2</v>
+        <v>168</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B190" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C190">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -3535,38 +3530,38 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B191" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C191">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B192" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="C192">
         <v>2013</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B193" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C193">
         <v>2013</v>
@@ -3577,38 +3572,38 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B194" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C194">
         <v>2013</v>
       </c>
       <c r="D194">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="B195" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="C195">
         <v>2013</v>
       </c>
       <c r="D195">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="B196" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="C196">
         <v>2013</v>
@@ -3619,41 +3614,41 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B197" t="s">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="C197">
         <v>2013</v>
       </c>
       <c r="D197">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B198" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C198">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D198">
-        <v>164</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B199" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="C199">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D199">
         <v>1</v>
@@ -3661,27 +3656,27 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B200" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="C200">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D200">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B201" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C201">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D201">
         <v>1</v>
@@ -3689,13 +3684,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C202">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D202">
         <v>2</v>
@@ -3703,13 +3698,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C203">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D203">
         <v>1</v>
@@ -3717,13 +3712,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B204" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="C204">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D204">
         <v>1</v>
@@ -3731,13 +3726,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B205" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C205">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D205">
         <v>1</v>
@@ -3745,10 +3740,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B206" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C206">
         <v>2012</v>
@@ -3759,66 +3754,66 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B207" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="C207">
         <v>2012</v>
       </c>
       <c r="D207">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B208" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="C208">
         <v>2012</v>
       </c>
       <c r="D208">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="B209" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="C209">
         <v>2012</v>
       </c>
       <c r="D209">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B210" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C210">
         <v>2012</v>
       </c>
       <c r="D210">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="B211" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="C211">
         <v>2012</v>
@@ -3829,10 +3824,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B212" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="C212">
         <v>2012</v>
@@ -3843,24 +3838,24 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="B213" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="C213">
         <v>2012</v>
       </c>
       <c r="D213">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="B214" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C214">
         <v>2012</v>
@@ -3871,27 +3866,27 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="B215" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C215">
         <v>2012</v>
       </c>
       <c r="D215">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B216" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C216">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -3899,13 +3894,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="B217" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C217">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D217">
         <v>1</v>
@@ -3913,13 +3908,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="B218" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="C218">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -3927,13 +3922,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="B219" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="C219">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -3941,13 +3936,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="B220" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C220">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -3955,13 +3950,13 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B221" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C221">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D221">
         <v>1</v>
@@ -3969,10 +3964,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B222" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C222">
         <v>2011</v>
@@ -3983,13 +3978,13 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B223" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C223">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D223">
         <v>1</v>
@@ -3997,13 +3992,13 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="B224" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C224">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D224">
         <v>1</v>
@@ -4011,13 +4006,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="B225" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="C225">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D225">
         <v>1</v>
@@ -4025,13 +4020,13 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B226" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C226">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="D226">
         <v>1</v>
@@ -4039,13 +4034,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B227" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C227">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="D227">
         <v>1</v>
@@ -4053,13 +4048,13 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B228" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C228">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="D228">
         <v>1</v>
@@ -4067,13 +4062,13 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B229" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C229">
-        <v>2009</v>
+        <v>1991</v>
       </c>
       <c r="D229">
         <v>1</v>
@@ -4081,99 +4076,15 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B230" t="s">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="C230">
-        <v>2007</v>
+        <v>1989</v>
       </c>
       <c r="D230">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>156</v>
-      </c>
-      <c r="B231" t="s">
-        <v>24</v>
-      </c>
-      <c r="C231">
-        <v>2007</v>
-      </c>
-      <c r="D231">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>60</v>
-      </c>
-      <c r="B232" t="s">
-        <v>157</v>
-      </c>
-      <c r="C232">
-        <v>2006</v>
-      </c>
-      <c r="D232">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>10</v>
-      </c>
-      <c r="B233" t="s">
-        <v>11</v>
-      </c>
-      <c r="C233">
-        <v>2005</v>
-      </c>
-      <c r="D233">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>67</v>
-      </c>
-      <c r="B234" t="s">
-        <v>158</v>
-      </c>
-      <c r="C234">
-        <v>2005</v>
-      </c>
-      <c r="D234">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>67</v>
-      </c>
-      <c r="B235" t="s">
-        <v>159</v>
-      </c>
-      <c r="C235">
-        <v>1991</v>
-      </c>
-      <c r="D235">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>10</v>
-      </c>
-      <c r="B236" t="s">
-        <v>82</v>
-      </c>
-      <c r="C236">
-        <v>1989</v>
-      </c>
-      <c r="D236">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update mileage and fuel economy assignment
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiaru\Documents\UiPath\762-impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somet\Documents\Engineering\PartIV\762-impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D275A6-E329-4561-AAD4-F34A4E2DFF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D183E879-E623-4D1C-A3A1-39A0DF03F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{4A75A796-F6A9-442D-AA11-4067559B62C0}"/>
+    <workbookView xWindow="17685" yWindow="4515" windowWidth="32505" windowHeight="15345" xr2:uid="{9F670307-BB0C-410C-A732-BF2E1B69CA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="167">
   <si>
     <t>Make</t>
   </si>
@@ -69,6 +71,18 @@
     <t>multivan</t>
   </si>
   <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t>prius</t>
+  </si>
+  <si>
+    <t>land-cruiser</t>
+  </si>
+  <si>
+    <t>hilux</t>
+  </si>
+  <si>
     <t>tesla</t>
   </si>
   <si>
@@ -222,18 +236,12 @@
     <t>t-roc</t>
   </si>
   <si>
-    <t>toyota</t>
-  </si>
-  <si>
     <t>yaris</t>
   </si>
   <si>
     <t>rav4</t>
   </si>
   <si>
-    <t>prius</t>
-  </si>
-  <si>
     <t>mercedes-benz</t>
   </si>
   <si>
@@ -249,9 +257,6 @@
     <t>raize</t>
   </si>
   <si>
-    <t>hilux</t>
-  </si>
-  <si>
     <t>suzuki</t>
   </si>
   <si>
@@ -267,6 +272,12 @@
     <t>juke</t>
   </si>
   <si>
+    <t>honda</t>
+  </si>
+  <si>
+    <t>hr-v</t>
+  </si>
+  <si>
     <t>530e</t>
   </si>
   <si>
@@ -303,6 +314,9 @@
     <t>range-rover-sport</t>
   </si>
   <si>
+    <t>seltos</t>
+  </si>
+  <si>
     <t>tucson</t>
   </si>
   <si>
@@ -357,6 +371,12 @@
     <t>c-350-e</t>
   </si>
   <si>
+    <t>holden</t>
+  </si>
+  <si>
+    <t>astra</t>
+  </si>
+  <si>
     <t>territory</t>
   </si>
   <si>
@@ -372,6 +392,9 @@
     <t>passat</t>
   </si>
   <si>
+    <t>land-cruiser-prado</t>
+  </si>
+  <si>
     <t>audi</t>
   </si>
   <si>
@@ -381,6 +404,9 @@
     <t>jetta</t>
   </si>
   <si>
+    <t>outback</t>
+  </si>
+  <si>
     <t>macan</t>
   </si>
   <si>
@@ -402,13 +428,16 @@
     <t>rc-300</t>
   </si>
   <si>
+    <t>nx-300h</t>
+  </si>
+  <si>
     <t>jaguar</t>
   </si>
   <si>
     <t>xf</t>
   </si>
   <si>
-    <t>holden</t>
+    <t>grace</t>
   </si>
   <si>
     <t>colorado</t>
@@ -420,24 +449,21 @@
     <t>i8</t>
   </si>
   <si>
+    <t>435i</t>
+  </si>
+  <si>
     <t>a4</t>
   </si>
   <si>
-    <t>harrier</t>
-  </si>
-  <si>
     <t>cx-9</t>
   </si>
   <si>
-    <t>nx-300h</t>
-  </si>
-  <si>
-    <t>honda</t>
-  </si>
-  <si>
     <t>vezel</t>
   </si>
   <si>
+    <t>116i</t>
+  </si>
+  <si>
     <t>sq5</t>
   </si>
   <si>
@@ -483,7 +509,7 @@
     <t>x3</t>
   </si>
   <si>
-    <t>116i</t>
+    <t>328i</t>
   </si>
   <si>
     <t>fit</t>
@@ -861,8 +887,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C06B43-F583-4687-B11F-98B0E0DF934B}">
-  <dimension ref="A1:D230"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2F4298-1953-427F-A2F4-DB0B52842867}">
+  <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -935,7 +961,7 @@
         <v>2022</v>
       </c>
       <c r="D5">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,24 +980,24 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2022</v>
@@ -982,21 +1008,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
       <c r="C9">
         <v>2022</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -1005,12 +1031,12 @@
         <v>2022</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1019,77 +1045,77 @@
         <v>2022</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>2022</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>3008</v>
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
       </c>
       <c r="C13">
         <v>2022</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>2022</v>
       </c>
       <c r="D14">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>2022</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>3008</v>
       </c>
       <c r="C16">
         <v>2022</v>
       </c>
       <c r="D16">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,13 +1123,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>2022</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1137,13 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>2022</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,13 +1151,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>2022</v>
       </c>
       <c r="D19">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,18 +1165,18 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>2022</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -1159,40 +1185,40 @@
         <v>2022</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
         <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
       </c>
       <c r="C22">
         <v>2022</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>2022</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
@@ -1201,7 +1227,7 @@
         <v>2022</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,7 +1241,7 @@
         <v>2022</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1229,26 +1255,26 @@
         <v>2022</v>
       </c>
       <c r="D26">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
         <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
       </c>
       <c r="C27">
         <v>2022</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
@@ -1257,26 +1283,26 @@
         <v>2022</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
         <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
       </c>
       <c r="C29">
         <v>2022</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
         <v>42</v>
@@ -1290,7 +1316,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
@@ -1299,15 +1325,15 @@
         <v>2022</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32">
         <v>2022</v>
@@ -1318,38 +1344,38 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33">
         <v>2022</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>2022</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>2022</v>
@@ -1360,21 +1386,21 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36">
         <v>2022</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -1383,12 +1409,12 @@
         <v>2022</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
@@ -1397,12 +1423,12 @@
         <v>2022</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
@@ -1425,43 +1451,43 @@
         <v>2022</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
         <v>55</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
       </c>
       <c r="C41">
         <v>2022</v>
       </c>
       <c r="D41">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C42">
         <v>2022</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43">
         <v>2022</v>
@@ -1472,41 +1498,41 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="B45" t="s">
-        <v>63</v>
-      </c>
       <c r="C45">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
         <v>64</v>
       </c>
       <c r="C46">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1514,7 +1540,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
@@ -1523,15 +1549,15 @@
         <v>2021</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C48">
         <v>2021</v>
@@ -1542,10 +1568,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49">
-        <v>508</v>
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
       </c>
       <c r="C49">
         <v>2021</v>
@@ -1556,52 +1582,52 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C50">
         <v>2021</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C51">
         <v>2021</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C52">
         <v>2021</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" t="s">
-        <v>67</v>
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>508</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -1612,52 +1638,52 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C54">
         <v>2021</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C55">
         <v>2021</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="C56">
         <v>2021</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1668,41 +1694,41 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C58">
         <v>2021</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C59">
         <v>2021</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C60">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1710,13 +1736,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C61">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -1724,27 +1750,27 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C62">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C63">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -1752,10 +1778,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C64">
         <v>2020</v>
@@ -1766,80 +1792,80 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="C66">
         <v>2020</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="C67">
         <v>2020</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C68">
         <v>2020</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C69">
         <v>2020</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>28</v>
-      </c>
-      <c r="B70">
-        <v>3</v>
+        <v>75</v>
+      </c>
+      <c r="B70" t="s">
+        <v>77</v>
       </c>
       <c r="C70">
         <v>2020</v>
@@ -1850,24 +1876,24 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C71">
         <v>2020</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C72">
         <v>2020</v>
@@ -1878,55 +1904,55 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C73">
         <v>2020</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>6</v>
-      </c>
-      <c r="B74" t="s">
-        <v>78</v>
+        <v>32</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
       </c>
       <c r="C74">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C75">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D75">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B76" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C76">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -1934,66 +1960,66 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C77">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C78">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C79">
         <v>2019</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C80">
         <v>2019</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="C81">
         <v>2019</v>
@@ -2004,24 +2030,24 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>2019</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C83">
         <v>2019</v>
@@ -2032,24 +2058,24 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="C84">
         <v>2019</v>
       </c>
       <c r="D84">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C85">
         <v>2019</v>
@@ -2060,10 +2086,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C86">
         <v>2019</v>
@@ -2074,7 +2100,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>87</v>
@@ -2088,24 +2114,24 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <v>3</v>
+        <v>75</v>
+      </c>
+      <c r="B88" t="s">
+        <v>88</v>
       </c>
       <c r="C88">
         <v>2019</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C89">
         <v>2019</v>
@@ -2116,24 +2142,24 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>2019</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="C91">
         <v>2019</v>
@@ -2144,21 +2170,21 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C92">
         <v>2019</v>
       </c>
       <c r="D92">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B93" t="s">
         <v>90</v>
@@ -2172,27 +2198,27 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>57</v>
-      </c>
-      <c r="B94" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
       </c>
       <c r="C94">
         <v>2019</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C95">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -2200,83 +2226,83 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B96" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C96">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C97">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B98" t="s">
         <v>93</v>
       </c>
       <c r="C98">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="C99">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B100" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C100">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D100">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B101" t="s">
         <v>95</v>
       </c>
       <c r="C101">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -2284,7 +2310,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
         <v>96</v>
@@ -2293,15 +2319,15 @@
         <v>2018</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C103">
         <v>2018</v>
@@ -2312,10 +2338,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C104">
         <v>2018</v>
@@ -2326,24 +2352,24 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C105">
         <v>2018</v>
       </c>
       <c r="D105">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C106">
         <v>2018</v>
@@ -2354,21 +2380,21 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" t="s">
         <v>97</v>
-      </c>
-      <c r="B107" t="s">
-        <v>56</v>
       </c>
       <c r="C107">
         <v>2018</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B108" t="s">
         <v>98</v>
@@ -2382,10 +2408,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C109">
         <v>2018</v>
@@ -2396,24 +2422,24 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C110">
         <v>2018</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C111">
         <v>2018</v>
@@ -2424,24 +2450,24 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="C112">
         <v>2018</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B113" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C113">
         <v>2018</v>
@@ -2452,97 +2478,97 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C114">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
       <c r="C115">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D115">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C116">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="B117" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C117">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D117">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="B118" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="C118">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="B119" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C119">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D119">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="B120" t="s">
         <v>104</v>
       </c>
       <c r="C120">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -2550,27 +2576,27 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C121">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B122" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C122">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -2578,13 +2604,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B123" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C123">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -2592,7 +2618,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
         <v>105</v>
@@ -2601,15 +2627,15 @@
         <v>2017</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C125">
         <v>2017</v>
@@ -2620,122 +2646,122 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C126">
         <v>2017</v>
       </c>
       <c r="D126">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C127">
         <v>2017</v>
       </c>
       <c r="D127">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="C128">
         <v>2017</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C129">
         <v>2017</v>
       </c>
       <c r="D129">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B130" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C130">
         <v>2017</v>
       </c>
       <c r="D130">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B131" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="C131">
         <v>2017</v>
       </c>
       <c r="D131">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>85</v>
+      </c>
+      <c r="B132" t="s">
         <v>86</v>
-      </c>
-      <c r="B132">
-        <v>6</v>
       </c>
       <c r="C132">
         <v>2017</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B133" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C133">
         <v>2017</v>
       </c>
       <c r="D133">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B134" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C134">
         <v>2017</v>
@@ -2746,10 +2772,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B135" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C135">
         <v>2017</v>
@@ -2760,240 +2786,240 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="C136">
         <v>2017</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C137">
         <v>2017</v>
       </c>
       <c r="D137">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B138" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="C138">
         <v>2017</v>
       </c>
       <c r="D138">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B139" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C139">
         <v>2017</v>
       </c>
       <c r="D139">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="B140" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C140">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B141" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C141">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D141">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>9</v>
-      </c>
-      <c r="B142" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="B142">
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D142">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B143" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C143">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D143">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="B144" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C144">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B145" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C145">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C146">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D146">
-        <v>52</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B147" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C147">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D147">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B148" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C148">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D148">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B149" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C149">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D149">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B150" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C150">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D150">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C151">
         <v>2016</v>
       </c>
       <c r="D151">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C152">
         <v>2016</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3001,38 +3027,38 @@
         <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C153">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B154" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C154">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D154">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B155" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="C155">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -3040,13 +3066,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B156" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="C156">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -3054,13 +3080,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C157">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D157">
         <v>1</v>
@@ -3068,97 +3094,97 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="B158" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="C158">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D158">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C159">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D159">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="C160">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B161" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="C161">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B162" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C162">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="B163" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C163">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B164" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C164">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -3166,10 +3192,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B165" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="C165">
         <v>2015</v>
@@ -3180,24 +3206,24 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="B166" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C166">
         <v>2015</v>
       </c>
       <c r="D166">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B167" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C167">
         <v>2015</v>
@@ -3208,10 +3234,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B168" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="C168">
         <v>2015</v>
@@ -3222,10 +3248,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B169" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C169">
         <v>2015</v>
@@ -3236,10 +3262,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B170" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C170">
         <v>2015</v>
@@ -3250,55 +3276,55 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B171" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C171">
         <v>2015</v>
       </c>
       <c r="D171">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C172">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D172">
-        <v>1</v>
+        <v>116</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B173" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="C173">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D173">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C174">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D174">
         <v>1</v>
@@ -3306,27 +3332,27 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="C175">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D175">
-        <v>104</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="B176" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C176">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D176">
         <v>1</v>
@@ -3334,13 +3360,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B177" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C177">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D177">
         <v>1</v>
@@ -3348,27 +3374,27 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>131</v>
+      </c>
+      <c r="B178" t="s">
         <v>132</v>
       </c>
-      <c r="B178" t="s">
-        <v>133</v>
-      </c>
       <c r="C178">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D178">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="B179" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="C179">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D179">
         <v>1</v>
@@ -3376,13 +3402,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B180" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C180">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D180">
         <v>1</v>
@@ -3390,13 +3416,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="B181" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="C181">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -3404,13 +3430,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B182" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C182">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -3418,13 +3444,13 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B183" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="C183">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -3432,41 +3458,41 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B184" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C184">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D184">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B185" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="C185">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D185">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B186" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="C186">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -3474,27 +3500,27 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B187" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C187">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="D187">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B188" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C188">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D188">
         <v>1</v>
@@ -3502,41 +3528,41 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B189" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C189">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D189">
-        <v>168</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="C190">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D190">
-        <v>1</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B191" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C191">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -3544,27 +3570,27 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B192" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C192">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D192">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B193" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="C193">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -3572,13 +3598,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="B194" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="C194">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -3586,13 +3612,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="B195" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="C195">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D195">
         <v>2</v>
@@ -3600,10 +3626,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="B196" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="C196">
         <v>2013</v>
@@ -3614,69 +3640,69 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B197" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="C197">
         <v>2013</v>
       </c>
       <c r="D197">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B198" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C198">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D198">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B199" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="C199">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D199">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B200" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C200">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D200">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="B201" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C201">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D201">
         <v>1</v>
@@ -3684,16 +3710,16 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B202" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="C202">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D202">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3701,10 +3727,10 @@
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C203">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D203">
         <v>1</v>
@@ -3712,27 +3738,27 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>142</v>
+        <v>5</v>
       </c>
       <c r="C204">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D204">
-        <v>1</v>
+        <v>169</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B205" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C205">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D205">
         <v>1</v>
@@ -3740,13 +3766,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B206" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C206">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D206">
         <v>1</v>
@@ -3754,27 +3780,27 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B207" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C207">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D207">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="B208" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="C208">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D208">
         <v>1</v>
@@ -3782,41 +3808,41 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="B209" t="s">
-        <v>147</v>
+        <v>36</v>
       </c>
       <c r="C209">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D209">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B210" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C210">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D210">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B211" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="C211">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -3824,27 +3850,27 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B212" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C212">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D212">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B213" t="s">
-        <v>58</v>
+        <v>141</v>
       </c>
       <c r="C213">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D213">
         <v>1</v>
@@ -3852,24 +3878,24 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B214" t="s">
-        <v>148</v>
+        <v>8</v>
       </c>
       <c r="C214">
         <v>2012</v>
       </c>
       <c r="D214">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B215" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="C215">
         <v>2012</v>
@@ -3880,55 +3906,55 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B216" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C216">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D216">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B217" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C217">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D217">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="B218" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="C218">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D218">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>122</v>
+        <v>4</v>
       </c>
       <c r="B219" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="C219">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -3936,13 +3962,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="B220" t="s">
         <v>150</v>
       </c>
       <c r="C220">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -3950,13 +3976,13 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B221" t="s">
         <v>151</v>
       </c>
       <c r="C221">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D221">
         <v>1</v>
@@ -3964,13 +3990,13 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B222" t="s">
         <v>152</v>
       </c>
       <c r="C222">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D222">
         <v>1</v>
@@ -3978,27 +4004,27 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="B223" t="s">
         <v>153</v>
       </c>
       <c r="C223">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D223">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="B224" t="s">
         <v>154</v>
       </c>
       <c r="C224">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D224">
         <v>1</v>
@@ -4006,27 +4032,27 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="B225" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="C225">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="D225">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B226" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
       <c r="C226">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="D226">
         <v>1</v>
@@ -4034,13 +4060,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B227" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="C227">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="D227">
         <v>1</v>
@@ -4048,13 +4074,13 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B228" t="s">
-        <v>157</v>
+        <v>46</v>
       </c>
       <c r="C228">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="D228">
         <v>1</v>
@@ -4062,13 +4088,13 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B229" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="C229">
-        <v>1991</v>
+        <v>2012</v>
       </c>
       <c r="D229">
         <v>1</v>
@@ -4076,15 +4102,281 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>61</v>
+      </c>
+      <c r="B230" t="s">
+        <v>156</v>
+      </c>
+      <c r="C230">
+        <v>2012</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>61</v>
+      </c>
+      <c r="B231" t="s">
+        <v>157</v>
+      </c>
+      <c r="C231">
+        <v>2012</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>61</v>
+      </c>
+      <c r="B232" t="s">
+        <v>141</v>
+      </c>
+      <c r="C232">
+        <v>2012</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>9</v>
+      </c>
+      <c r="B233" t="s">
+        <v>105</v>
+      </c>
+      <c r="C233">
+        <v>2011</v>
+      </c>
+      <c r="D233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>9</v>
+      </c>
+      <c r="B234" t="s">
+        <v>116</v>
+      </c>
+      <c r="C234">
+        <v>2011</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>128</v>
+      </c>
+      <c r="B235" t="s">
+        <v>153</v>
+      </c>
+      <c r="C235">
+        <v>2011</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>131</v>
+      </c>
+      <c r="B236" t="s">
+        <v>132</v>
+      </c>
+      <c r="C236">
+        <v>2011</v>
+      </c>
+      <c r="D236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>78</v>
+      </c>
+      <c r="B237" t="s">
+        <v>158</v>
+      </c>
+      <c r="C237">
+        <v>2011</v>
+      </c>
+      <c r="D237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>53</v>
+      </c>
+      <c r="B238" t="s">
+        <v>159</v>
+      </c>
+      <c r="C238">
+        <v>2011</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>61</v>
+      </c>
+      <c r="B239" t="s">
+        <v>160</v>
+      </c>
+      <c r="C239">
+        <v>2011</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>128</v>
+      </c>
+      <c r="B240" t="s">
+        <v>153</v>
+      </c>
+      <c r="C240">
+        <v>2010</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>75</v>
+      </c>
+      <c r="B241" t="s">
+        <v>161</v>
+      </c>
+      <c r="C241">
+        <v>2009</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>61</v>
+      </c>
+      <c r="B242" t="s">
+        <v>162</v>
+      </c>
+      <c r="C242">
+        <v>2009</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>61</v>
+      </c>
+      <c r="B243" t="s">
         <v>62</v>
       </c>
-      <c r="B230" t="s">
-        <v>80</v>
-      </c>
-      <c r="C230">
+      <c r="C243">
+        <v>2008</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>73</v>
+      </c>
+      <c r="B244" t="s">
+        <v>163</v>
+      </c>
+      <c r="C244">
+        <v>2007</v>
+      </c>
+      <c r="D244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>61</v>
+      </c>
+      <c r="B245" t="s">
+        <v>164</v>
+      </c>
+      <c r="C245">
+        <v>2006</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>11</v>
+      </c>
+      <c r="B246" t="s">
+        <v>13</v>
+      </c>
+      <c r="C246">
+        <v>2005</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>68</v>
+      </c>
+      <c r="B247" t="s">
+        <v>165</v>
+      </c>
+      <c r="C247">
+        <v>2005</v>
+      </c>
+      <c r="D247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>68</v>
+      </c>
+      <c r="B248" t="s">
+        <v>166</v>
+      </c>
+      <c r="C248">
+        <v>1991</v>
+      </c>
+      <c r="D248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>11</v>
+      </c>
+      <c r="B249" t="s">
+        <v>83</v>
+      </c>
+      <c r="C249">
         <v>1989</v>
       </c>
-      <c r="D230">
+      <c r="D249">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
review app, update readme, make new release
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somet\Documents\Engineering\PartIV\762-impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\762-impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D183E879-E623-4D1C-A3A1-39A0DF03F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AD242F-A479-486C-B1FA-BB93C7888064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17685" yWindow="4515" windowWidth="32505" windowHeight="15345" xr2:uid="{9F670307-BB0C-410C-A732-BF2E1B69CA96}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12645" xr2:uid="{F4AC49F4-BBE0-4A8D-9EBA-1455D555BCD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="167">
   <si>
     <t>Make</t>
   </si>
@@ -543,12 +543,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -570,13 +578,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -592,7 +604,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -887,14 +899,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2F4298-1953-427F-A2F4-DB0B52842867}">
-  <dimension ref="A1:D249"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7B83B8-4ECE-4B4C-BCF9-6472CB60EB2B}">
+  <dimension ref="A1:D248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -922,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -936,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -950,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -964,7 +976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -978,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1115,10 +1127,10 @@
         <v>2022</v>
       </c>
       <c r="D16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1157,10 +1169,10 @@
         <v>2022</v>
       </c>
       <c r="D19">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1199,10 +1211,10 @@
         <v>2022</v>
       </c>
       <c r="D22">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1227,10 +1239,10 @@
         <v>2022</v>
       </c>
       <c r="D24">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1272,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1283,10 +1295,10 @@
         <v>2022</v>
       </c>
       <c r="D28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1300,7 +1312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1314,7 +1326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1328,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1342,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1398,7 +1410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -1496,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -1510,7 +1522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -1538,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1552,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -1594,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1608,12 +1620,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>508</v>
       </c>
       <c r="C52">
         <v>2021</v>
@@ -1622,82 +1634,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53">
-        <v>508</v>
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
       </c>
       <c r="C53">
         <v>2021</v>
       </c>
       <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C54">
         <v>2021</v>
       </c>
       <c r="D54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C55">
         <v>2021</v>
       </c>
       <c r="D55">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C56">
         <v>2021</v>
       </c>
       <c r="D56">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="C57">
         <v>2021</v>
       </c>
       <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1706,26 +1718,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C59">
         <v>2021</v>
       </c>
       <c r="D59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1734,12 +1746,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1748,40 +1760,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C62">
         <v>2021</v>
       </c>
       <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C63">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>2020</v>
@@ -1790,40 +1802,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C66">
         <v>2020</v>
       </c>
       <c r="D66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1832,68 +1844,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C68">
         <v>2020</v>
       </c>
       <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>2020</v>
       </c>
       <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>75</v>
-      </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="C70">
         <v>2020</v>
       </c>
       <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C71">
         <v>2020</v>
       </c>
       <c r="D71">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C72">
         <v>2020</v>
@@ -1902,26 +1914,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
       </c>
       <c r="C73">
         <v>2020</v>
       </c>
       <c r="D73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>32</v>
-      </c>
-      <c r="B74">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="B74" t="s">
+        <v>40</v>
       </c>
       <c r="C74">
         <v>2020</v>
@@ -1930,26 +1942,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C75">
         <v>2020</v>
       </c>
       <c r="D75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -1958,12 +1970,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C77">
         <v>2020</v>
@@ -1972,110 +1984,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C78">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C79">
         <v>2019</v>
       </c>
       <c r="D79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C80">
         <v>2019</v>
       </c>
       <c r="D80">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C81">
         <v>2019</v>
       </c>
       <c r="D81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C82">
         <v>2019</v>
       </c>
       <c r="D82">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C83">
         <v>2019</v>
       </c>
       <c r="D83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C84">
         <v>2019</v>
       </c>
       <c r="D84">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C85">
         <v>2019</v>
@@ -2084,12 +2096,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C86">
         <v>2019</v>
@@ -2098,12 +2110,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C87">
         <v>2019</v>
@@ -2112,12 +2124,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C88">
         <v>2019</v>
@@ -2126,40 +2138,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>2019</v>
       </c>
       <c r="D89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C90">
         <v>2019</v>
       </c>
       <c r="D90">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C91">
         <v>2019</v>
@@ -2168,12 +2180,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C92">
         <v>2019</v>
@@ -2182,40 +2194,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>89</v>
       </c>
-      <c r="B93" t="s">
-        <v>90</v>
+      <c r="B93">
+        <v>3</v>
       </c>
       <c r="C93">
         <v>2019</v>
       </c>
       <c r="D93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>89</v>
-      </c>
-      <c r="B94">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="B94" t="s">
+        <v>91</v>
       </c>
       <c r="C94">
         <v>2019</v>
       </c>
       <c r="D94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B95" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C95">
         <v>2019</v>
@@ -2224,12 +2236,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>38</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C96">
         <v>2019</v>
@@ -2238,12 +2250,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="C97">
         <v>2019</v>
@@ -2252,40 +2264,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>44</v>
       </c>
       <c r="B98" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="C98">
         <v>2019</v>
       </c>
       <c r="D98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="C99">
         <v>2019</v>
       </c>
       <c r="D99">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C100">
         <v>2019</v>
@@ -2294,26 +2306,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C101">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C102">
         <v>2018</v>
@@ -2322,40 +2334,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C103">
         <v>2018</v>
       </c>
       <c r="D103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C104">
         <v>2018</v>
       </c>
       <c r="D104">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C105">
         <v>2018</v>
@@ -2364,26 +2376,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="C106">
         <v>2018</v>
       </c>
       <c r="D106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C107">
         <v>2018</v>
@@ -2392,54 +2404,54 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C108">
         <v>2018</v>
       </c>
       <c r="D108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C109">
         <v>2018</v>
       </c>
       <c r="D109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C110">
         <v>2018</v>
       </c>
       <c r="D110">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C111">
         <v>2018</v>
@@ -2448,68 +2460,68 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B112" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C112">
         <v>2018</v>
       </c>
       <c r="D112">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>75</v>
       </c>
       <c r="B113" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C113">
         <v>2018</v>
       </c>
       <c r="D113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="C114">
         <v>2018</v>
       </c>
       <c r="D114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C115">
         <v>2018</v>
       </c>
       <c r="D115">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="B116" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C116">
         <v>2018</v>
@@ -2518,40 +2530,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>101</v>
       </c>
       <c r="B117" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="C117">
         <v>2018</v>
       </c>
       <c r="D117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>101</v>
       </c>
       <c r="B118" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C118">
         <v>2018</v>
       </c>
       <c r="D118">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="B119" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C119">
         <v>2018</v>
@@ -2560,40 +2572,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C120">
         <v>2018</v>
       </c>
       <c r="D120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>44</v>
       </c>
       <c r="B121" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="C121">
         <v>2018</v>
       </c>
       <c r="D121">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="C122">
         <v>2018</v>
@@ -2602,110 +2614,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C123">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D123">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B124" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C124">
         <v>2017</v>
       </c>
       <c r="D124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="C125">
         <v>2017</v>
       </c>
       <c r="D125">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C126">
         <v>2017</v>
       </c>
       <c r="D126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C127">
         <v>2017</v>
       </c>
       <c r="D127">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C128">
         <v>2017</v>
       </c>
       <c r="D128">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B129" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C129">
         <v>2017</v>
       </c>
       <c r="D129">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="C130">
         <v>2017</v>
@@ -2714,12 +2726,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B131" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="C131">
         <v>2017</v>
@@ -2728,26 +2740,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B132" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C132">
         <v>2017</v>
       </c>
       <c r="D132">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>75</v>
       </c>
       <c r="B133" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="C133">
         <v>2017</v>
@@ -2756,152 +2768,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>75</v>
       </c>
       <c r="B134" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C134">
         <v>2017</v>
       </c>
       <c r="D134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="C135">
         <v>2017</v>
       </c>
       <c r="D135">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C136">
         <v>2017</v>
       </c>
       <c r="D136">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="B137" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C137">
         <v>2017</v>
       </c>
       <c r="D137">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>101</v>
       </c>
       <c r="B138" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="C138">
         <v>2017</v>
       </c>
       <c r="D138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>101</v>
       </c>
       <c r="B139" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C139">
         <v>2017</v>
       </c>
       <c r="D139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="B140" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C140">
         <v>2017</v>
       </c>
       <c r="D140">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>68</v>
-      </c>
-      <c r="B141" t="s">
-        <v>110</v>
+        <v>89</v>
+      </c>
+      <c r="B141">
+        <v>6</v>
       </c>
       <c r="C141">
         <v>2017</v>
       </c>
       <c r="D141">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>89</v>
-      </c>
-      <c r="B142">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="B142" t="s">
+        <v>46</v>
       </c>
       <c r="C142">
         <v>2017</v>
       </c>
       <c r="D142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B143" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="C143">
         <v>2017</v>
       </c>
       <c r="D143">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B144" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C144">
         <v>2017</v>
@@ -2910,26 +2922,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B145" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="C145">
         <v>2017</v>
       </c>
       <c r="D145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>61</v>
       </c>
       <c r="B146" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="C146">
         <v>2017</v>
@@ -2938,110 +2950,110 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>61</v>
       </c>
       <c r="B147" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C147">
         <v>2017</v>
       </c>
       <c r="D147">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>61</v>
       </c>
       <c r="B148" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="C148">
         <v>2017</v>
       </c>
       <c r="D148">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>61</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C149">
         <v>2017</v>
       </c>
       <c r="D149">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C150">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D150">
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C151">
         <v>2016</v>
       </c>
       <c r="D151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C152">
         <v>2016</v>
       </c>
       <c r="D152">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B153" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C153">
         <v>2016</v>
       </c>
       <c r="D153">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>11</v>
       </c>
       <c r="B154" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="C154">
         <v>2016</v>
@@ -3050,12 +3062,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>11</v>
       </c>
       <c r="B155" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="C155">
         <v>2016</v>
@@ -3064,12 +3076,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>11</v>
       </c>
       <c r="B156" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C156">
         <v>2016</v>
@@ -3078,40 +3090,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C157">
         <v>2016</v>
       </c>
       <c r="D157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C158">
         <v>2016</v>
       </c>
       <c r="D158">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B159" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C159">
         <v>2016</v>
@@ -3120,12 +3132,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B160" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C160">
         <v>2016</v>
@@ -3134,26 +3146,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>61</v>
       </c>
       <c r="B161" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="C161">
         <v>2016</v>
       </c>
       <c r="D161">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>61</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C162">
         <v>2016</v>
@@ -3162,68 +3174,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B163" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C163">
         <v>2016</v>
       </c>
       <c r="D163">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="B164" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C164">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D164">
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>9</v>
       </c>
       <c r="B165" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C165">
         <v>2015</v>
       </c>
       <c r="D165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B166" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="C166">
         <v>2015</v>
       </c>
       <c r="D166">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>11</v>
       </c>
       <c r="B167" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C167">
         <v>2015</v>
@@ -3232,12 +3244,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B168" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="C168">
         <v>2015</v>
@@ -3246,26 +3258,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B169" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C169">
         <v>2015</v>
       </c>
       <c r="D169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B170" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C170">
         <v>2015</v>
@@ -3274,40 +3286,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C171">
         <v>2015</v>
       </c>
       <c r="D171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="C172">
         <v>2015</v>
       </c>
       <c r="D172">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>68</v>
       </c>
       <c r="B173" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C173">
         <v>2015</v>
@@ -3316,12 +3328,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C174">
         <v>2015</v>
@@ -3330,12 +3342,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="B175" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C175">
         <v>2015</v>
@@ -3344,12 +3356,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>128</v>
       </c>
       <c r="B176" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C176">
         <v>2015</v>
@@ -3358,12 +3370,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B177" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C177">
         <v>2015</v>
@@ -3372,12 +3384,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="B178" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="C178">
         <v>2015</v>
@@ -3386,12 +3398,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B179" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="C179">
         <v>2015</v>
@@ -3400,12 +3412,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="B180" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C180">
         <v>2015</v>
@@ -3414,12 +3426,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B181" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="C181">
         <v>2015</v>
@@ -3428,12 +3440,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>61</v>
       </c>
       <c r="B182" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="C182">
         <v>2015</v>
@@ -3442,12 +3454,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>61</v>
       </c>
       <c r="B183" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C183">
         <v>2015</v>
@@ -3456,12 +3468,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>61</v>
       </c>
       <c r="B184" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C184">
         <v>2015</v>
@@ -3470,12 +3482,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B185" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C185">
         <v>2015</v>
@@ -3484,110 +3496,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>119</v>
       </c>
       <c r="B186" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C186">
         <v>2015</v>
       </c>
       <c r="D186">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C187">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D187">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B188" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="C188">
         <v>2014</v>
       </c>
       <c r="D188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C189">
         <v>2014</v>
       </c>
       <c r="D189">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="C190">
         <v>2014</v>
       </c>
       <c r="D190">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B191" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C191">
         <v>2014</v>
       </c>
       <c r="D191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B192" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C192">
         <v>2014</v>
       </c>
       <c r="D192">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B193" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C193">
         <v>2014</v>
@@ -3596,40 +3608,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>119</v>
       </c>
       <c r="B194" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C194">
         <v>2014</v>
       </c>
       <c r="D194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="B195" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="C195">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D195">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>9</v>
       </c>
       <c r="B196" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C196">
         <v>2013</v>
@@ -3638,12 +3650,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B197" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C197">
         <v>2013</v>
@@ -3652,40 +3664,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>11</v>
       </c>
       <c r="B198" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C198">
         <v>2013</v>
       </c>
       <c r="D198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>11</v>
       </c>
       <c r="B199" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C199">
         <v>2013</v>
       </c>
       <c r="D199">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B200" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="C200">
         <v>2013</v>
@@ -3694,12 +3706,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="B201" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="C201">
         <v>2013</v>
@@ -3708,12 +3720,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C202">
         <v>2013</v>
@@ -3722,40 +3734,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="C203">
         <v>2013</v>
       </c>
       <c r="D203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B204" t="s">
-        <v>5</v>
+        <v>145</v>
       </c>
       <c r="C204">
         <v>2013</v>
       </c>
       <c r="D204">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>68</v>
       </c>
       <c r="B205" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C205">
         <v>2013</v>
@@ -3764,40 +3776,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B206" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C206">
         <v>2013</v>
       </c>
       <c r="D206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="B207" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="C207">
         <v>2013</v>
       </c>
       <c r="D207">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>34</v>
       </c>
       <c r="B208" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C208">
         <v>2013</v>
@@ -3806,124 +3818,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B209" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C209">
         <v>2013</v>
       </c>
       <c r="D209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="B210" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="C210">
         <v>2013</v>
       </c>
       <c r="D210">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B211" t="s">
-        <v>148</v>
+        <v>62</v>
       </c>
       <c r="C211">
         <v>2013</v>
       </c>
       <c r="D211">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>61</v>
       </c>
       <c r="B212" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="C212">
         <v>2013</v>
       </c>
       <c r="D212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>6</v>
+      </c>
+      <c r="B213" t="s">
+        <v>8</v>
+      </c>
+      <c r="C213">
+        <v>2012</v>
+      </c>
+      <c r="D213">
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>61</v>
-      </c>
-      <c r="B213" t="s">
-        <v>141</v>
-      </c>
-      <c r="C213">
-        <v>2013</v>
-      </c>
-      <c r="D213">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B214" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C214">
         <v>2012</v>
       </c>
       <c r="D214">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B215" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="C215">
         <v>2012</v>
       </c>
       <c r="D215">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>11</v>
       </c>
       <c r="B216" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C216">
         <v>2012</v>
       </c>
       <c r="D216">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C217">
         <v>2012</v>
@@ -3932,26 +3944,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>4</v>
       </c>
       <c r="B218" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="C218">
         <v>2012</v>
       </c>
       <c r="D218">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B219" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C219">
         <v>2012</v>
@@ -3960,12 +3972,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>68</v>
       </c>
       <c r="B220" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C220">
         <v>2012</v>
@@ -3974,12 +3986,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>68</v>
       </c>
       <c r="B221" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C221">
         <v>2012</v>
@@ -3988,68 +4000,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="B222" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C222">
         <v>2012</v>
       </c>
       <c r="D222">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>128</v>
       </c>
       <c r="B223" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C223">
         <v>2012</v>
       </c>
       <c r="D223">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>128</v>
       </c>
       <c r="B224" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C224">
         <v>2012</v>
       </c>
       <c r="D224">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="B225" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
       <c r="C225">
         <v>2012</v>
       </c>
       <c r="D225">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="B226" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="C226">
         <v>2012</v>
@@ -4058,12 +4070,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="B227" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="C227">
         <v>2012</v>
@@ -4072,12 +4084,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B228" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C228">
         <v>2012</v>
@@ -4086,12 +4098,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>61</v>
       </c>
       <c r="B229" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="C229">
         <v>2012</v>
@@ -4100,12 +4112,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>61</v>
       </c>
       <c r="B230" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C230">
         <v>2012</v>
@@ -4114,12 +4126,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>61</v>
       </c>
       <c r="B231" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C231">
         <v>2012</v>
@@ -4128,26 +4140,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B232" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C232">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D232">
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>9</v>
       </c>
       <c r="B233" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C233">
         <v>2011</v>
@@ -4156,12 +4168,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B234" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C234">
         <v>2011</v>
@@ -4170,12 +4182,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B235" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="C235">
         <v>2011</v>
@@ -4184,12 +4196,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="B236" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="C236">
         <v>2011</v>
@@ -4198,12 +4210,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B237" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C237">
         <v>2011</v>
@@ -4212,12 +4224,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B238" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C238">
         <v>2011</v>
@@ -4226,40 +4238,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
+        <v>128</v>
+      </c>
+      <c r="B239" t="s">
+        <v>153</v>
+      </c>
+      <c r="C239">
+        <v>2010</v>
+      </c>
+      <c r="D239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>75</v>
+      </c>
+      <c r="B240" t="s">
+        <v>161</v>
+      </c>
+      <c r="C240">
+        <v>2009</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
         <v>61</v>
       </c>
-      <c r="B239" t="s">
-        <v>160</v>
-      </c>
-      <c r="C239">
-        <v>2011</v>
-      </c>
-      <c r="D239">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>128</v>
-      </c>
-      <c r="B240" t="s">
-        <v>153</v>
-      </c>
-      <c r="C240">
-        <v>2010</v>
-      </c>
-      <c r="D240">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>75</v>
-      </c>
       <c r="B241" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C241">
         <v>2009</v>
@@ -4268,68 +4280,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>61</v>
       </c>
       <c r="B242" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="C242">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D242">
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>73</v>
+      </c>
+      <c r="B243" t="s">
+        <v>163</v>
+      </c>
+      <c r="C243">
+        <v>2007</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
         <v>61</v>
       </c>
-      <c r="B243" t="s">
-        <v>62</v>
-      </c>
-      <c r="C243">
-        <v>2008</v>
-      </c>
-      <c r="D243">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>73</v>
-      </c>
       <c r="B244" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C244">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D244">
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B245" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="C245">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D245">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B246" t="s">
-        <v>13</v>
+        <v>165</v>
       </c>
       <c r="C246">
         <v>2005</v>
@@ -4338,49 +4350,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>68</v>
       </c>
       <c r="B247" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C247">
-        <v>2005</v>
+        <v>1991</v>
       </c>
       <c r="D247">
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B248" t="s">
-        <v>166</v>
+        <v>83</v>
       </c>
       <c r="C248">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="D248">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>11</v>
-      </c>
-      <c r="B249" t="s">
-        <v>83</v>
-      </c>
-      <c r="C249">
-        <v>1989</v>
-      </c>
-      <c r="D249">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>